<commit_message>
protecting when log out
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XLS_ERP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901442A0-7567-4174-859C-9D0EEC4E3596}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC966AA-C77F-4C1B-8F41-835432A5E672}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="pWAswGgKw5fM41L682SgP0aaxIENytVFsMrm81ZY5I0z1LLjcTntoIFBAVhyMP9aa6iywLkmpmXEZrjU7Q7RiQ==" workbookSaltValue="U+lLYi7UkypWY+ltfx2ttg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16440" windowHeight="5180" xr2:uid="{DC68E485-ECDD-4095-A2ED-7BEBF6D9DF72}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16440" windowHeight="5180" firstSheet="2" activeTab="5" xr2:uid="{DC68E485-ECDD-4095-A2ED-7BEBF6D9DF72}"/>
   </bookViews>
   <sheets>
-    <sheet name="ERP_User_Table" sheetId="6" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="UserPermissionTable" sheetId="9" state="veryHidden" r:id="rId1"/>
+    <sheet name="UserPasswordTable" sheetId="7" state="veryHidden" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -34,33 +37,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Sheet 1</t>
-  </si>
-  <si>
-    <t>zhang</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>Li</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>zhang123</t>
-  </si>
-  <si>
-    <t>Li123</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>su2018</t>
+  </si>
+  <si>
+    <t>UserPasswordTable</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+  <si>
+    <t>Sheet3</t>
+  </si>
+  <si>
+    <t>UserPermissionTable</t>
+  </si>
+  <si>
+    <t>Writable</t>
+  </si>
+  <si>
+    <t>guest</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Invisible</t>
+  </si>
+  <si>
+    <t>Sheet4</t>
   </si>
 </sst>
 </file>
@@ -411,44 +429,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A555EC3-33E3-46BA-85CA-D722596EC5A2}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA05095-0F5A-4EC8-8B9C-48042AF4C69B}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:G1048576" xr:uid="{58B4B9F0-D121-4B2E-B43D-05F23C5FCFE0}">
+      <formula1>"Writable,ReadOnly,Invisible"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F1AAC9-2C18-4840-9AD7-4E47B78A53F3}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -457,7 +554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51E5B97-BC23-4FFE-AEC2-A4377E4FBBF8}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
@@ -466,12 +563,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
+  <sheetProtection algorithmName="SHA-512" hashValue="7S/l+q60lMcMPG8hD1nsjRSOmuTTd0nYAWlRldjAAx7EmXtVZJKdl2msm2gzmmofy825Yn48YZoWqgn4pLqmoQ==" saltValue="EzxoAoW8Vn1ipHstjahpoQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70249B5-FB2D-4A10-AA84-9B9DD62AEEFD}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
@@ -480,12 +578,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
+  <sheetProtection algorithmName="SHA-512" hashValue="WSYSxdWG621otIYWF+MgYvQbVrKNxHPQpSAjm5rYGu7OrVOQ8yrdatPOWhVM2QmS4XmF/MAq6R6zSxIXUzonkw==" saltValue="++2L8DGc4FfMF+dlEzRCSQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B481A777-A3DF-49D0-B403-B7DBF8503B65}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1"/>
@@ -493,7 +592,28 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="axEzRsiznBqcBBlTImzAfBkfn952kJRd8ugvC3ja6XVsGUE0yBbRM0Lf11k+gHjV4LLX6YIA10JveTPc7I5AWA==" saltValue="IRZzqSLGBUae6tvlsUGajQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFCE311-D1D2-4D9E-B15E-678C6A0E300A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
+  <sheetProtection algorithmName="SHA-512" hashValue="aj1rpAMUrI7EWpClQW/JIahV/5TEO81rofiXTC0+zL9Ss3f1ZltX23BYNUK2gmxs1DJV+gueC5kUDuTTsf6gSg==" saltValue="Bgwzi7mGxxDsgK9dXjVv5A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>